<commit_message>
transcriped Greg's functions into R code that does not require the SQLite background
</commit_message>
<xml_diff>
--- a/data/PITCleaner input files/Parent-Child Table RO 9-6-17.xlsx
+++ b/data/PITCleaner input files/Parent-Child Table RO 9-6-17.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RickO Sync\ISEMP 2017\PIT Cleaner\Input Data\INPUT Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryank\Documents\Ryan Sync\Collaborative Projects\DABOM\data\PITCleaner input files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -705,18 +705,6 @@
     <t>hatchery</t>
   </si>
   <si>
-    <t>Parent Array</t>
-  </si>
-  <si>
-    <t>Child Array</t>
-  </si>
-  <si>
-    <t>Basin or Branch</t>
-  </si>
-  <si>
-    <t>Obs Type</t>
-  </si>
-  <si>
     <t>Index</t>
   </si>
   <si>
@@ -727,6 +715,18 @@
   </si>
   <si>
     <t>BLTA0</t>
+  </si>
+  <si>
+    <t>ParentNode</t>
+  </si>
+  <si>
+    <t>ChildNode</t>
+  </si>
+  <si>
+    <t>MainBranch</t>
+  </si>
+  <si>
+    <t>SiteType</t>
   </si>
 </sst>
 </file>
@@ -1680,35 +1680,35 @@
   <dimension ref="A1:E208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="15.28515625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="9" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>230</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>73</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>73</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>88</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>91</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>91</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>91</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>91</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>93</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>94</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>94</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>89</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>95</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>87</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>85</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>86</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>90</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>73</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>181</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>182</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>213</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>178</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>178</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>181</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>70</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>69</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>102</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>100</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>181</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>114</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>174</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>188</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>148</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>149</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>175</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>176</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>63</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>62</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>61</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>176</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>176</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>170</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>169</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>167</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>167</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>165</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>73</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>118</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>117</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>116</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>120</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>191</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>190</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>189</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>206</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>116</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>119</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>150</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>73</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>103</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>104</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>110</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>110</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>103</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>105</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>103</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>103</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>81</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>103</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
         <v>73</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>126</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>73</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>73</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>48</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>66</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>73</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>45</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>73</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
         <v>73</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>73</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
         <v>138</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
         <v>71</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>73</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>9</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>8</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
         <v>6</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
         <v>7</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
         <v>7</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
         <v>3</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
         <v>5</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
         <v>3</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
         <v>4</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
         <v>4</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>73</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>99</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>97</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
         <v>73</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
         <v>75</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
         <v>73</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
         <v>76</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
         <v>42</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
         <v>41</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
         <v>32</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
         <v>32</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
         <v>32</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
         <v>32</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
         <v>32</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
         <v>32</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
         <v>32</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
         <v>76</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>73</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>205</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>205</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>205</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>140</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>205</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>73</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>144</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>147</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>145</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>146</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>154</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>152</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>153</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>201</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>200</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>196</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>194</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>195</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
         <v>73</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="16" t="s">
         <v>73</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="16" t="s">
         <v>59</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="16" t="s">
         <v>58</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="17" t="s">
         <v>73</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
         <v>157</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
         <v>155</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>73</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>172</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>198</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>158</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>158</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>158</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>158</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>198</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>68</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>198</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>199</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>212</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>43</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>198</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>203</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>204</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>198</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>184</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>187</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>187</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>73</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>20</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>73</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>132</v>
       </c>
@@ -4492,7 +4492,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>133</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>19</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>18</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>133</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>135</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>209</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>133</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>109</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>133</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>14</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>13</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>133</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>84</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>133</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>134</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>143</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>137</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>143</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>122</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>143</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>125</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>124</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>143</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>130</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>129</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>143</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>23</v>
       </c>
@@ -4951,12 +4951,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C193" s="2" t="s">
         <v>131</v>
@@ -4968,12 +4968,12 @@
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C194" s="2" t="s">
         <v>131</v>
@@ -4985,12 +4985,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C195" s="2" t="s">
         <v>131</v>
@@ -5002,9 +5002,9 @@
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B196" s="2" t="s">
         <v>25</v>
@@ -5019,7 +5019,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>25</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>28</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>26</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>27</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>143</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>31</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>143</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>80</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>79</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>143</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>2</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>1</v>
       </c>

</xml_diff>